<commit_message>
Add child care and food costs to income insufficiency
</commit_message>
<xml_diff>
--- a/data/raw_data/child_care/child_16_18.xlsx
+++ b/data/raw_data/child_care/child_16_18.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\staff\Documents\work_projects\indicators\i_income_insufficiency\data\raw_data\child_care\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\staff\Documents\work_projects\income-insufficiency\data\raw_data\child_care\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B240B664-06E4-40F2-92DF-2D5FC7389F8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{076448D2-A684-4381-8AEC-CDD25A47300A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" xr2:uid="{5529F818-3ED6-4855-A947-45FEBDFF3E60}"/>
   </bookViews>
@@ -405,13 +405,13 @@
     <t>school_Sthree</t>
   </si>
   <si>
-    <t>school_Sfoour</t>
-  </si>
-  <si>
     <t>shool_Sfive</t>
   </si>
   <si>
     <t>age_group</t>
+  </si>
+  <si>
+    <t>school_Sfour</t>
   </si>
 </sst>
 </file>
@@ -838,7 +838,7 @@
   <dimension ref="A1:C2601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +851,7 @@
         <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>572</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>594</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>412</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>427</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
         <v>383</v>
       </c>
       <c r="C78" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>393</v>
       </c>
       <c r="C79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>442</v>
       </c>
       <c r="C104" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1995,7 +1995,7 @@
         <v>468</v>
       </c>
       <c r="C105" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>449</v>
       </c>
       <c r="C130" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
         <v>488</v>
       </c>
       <c r="C131" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
         <v>422</v>
       </c>
       <c r="C156" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>430</v>
       </c>
       <c r="C157" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2842,7 +2842,7 @@
         <v>446</v>
       </c>
       <c r="C182" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>459</v>
       </c>
       <c r="C183" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>443</v>
       </c>
       <c r="C208" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -3139,7 +3139,7 @@
         <v>463</v>
       </c>
       <c r="C209" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>422</v>
       </c>
       <c r="C234" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>463</v>
       </c>
       <c r="C235" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>423</v>
       </c>
       <c r="C260" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3711,7 +3711,7 @@
         <v>431</v>
       </c>
       <c r="C261" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3986,7 +3986,7 @@
         <v>499</v>
       </c>
       <c r="C286" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3997,7 +3997,7 @@
         <v>541</v>
       </c>
       <c r="C287" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -4272,7 +4272,7 @@
         <v>401</v>
       </c>
       <c r="C312" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -4283,7 +4283,7 @@
         <v>436</v>
       </c>
       <c r="C313" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -4558,7 +4558,7 @@
         <v>475</v>
       </c>
       <c r="C338" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>492</v>
       </c>
       <c r="C339" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>403</v>
       </c>
       <c r="C364" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -4855,7 +4855,7 @@
         <v>426</v>
       </c>
       <c r="C365" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,7 +5130,7 @@
         <v>409</v>
       </c>
       <c r="C390" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -5141,7 +5141,7 @@
         <v>416</v>
       </c>
       <c r="C391" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
         <v>427</v>
       </c>
       <c r="C416" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -5427,7 +5427,7 @@
         <v>446</v>
       </c>
       <c r="C417" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
@@ -5702,7 +5702,7 @@
         <v>431</v>
       </c>
       <c r="C442" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
@@ -5713,7 +5713,7 @@
         <v>438</v>
       </c>
       <c r="C443" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
@@ -5988,7 +5988,7 @@
         <v>474</v>
       </c>
       <c r="C468" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -5999,7 +5999,7 @@
         <v>479</v>
       </c>
       <c r="C469" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
@@ -6274,7 +6274,7 @@
         <v>462</v>
       </c>
       <c r="C494" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
@@ -6285,7 +6285,7 @@
         <v>471</v>
       </c>
       <c r="C495" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
@@ -6560,7 +6560,7 @@
         <v>385</v>
       </c>
       <c r="C520" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -6571,7 +6571,7 @@
         <v>396</v>
       </c>
       <c r="C521" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
@@ -6846,7 +6846,7 @@
         <v>388</v>
       </c>
       <c r="C546" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
@@ -6857,7 +6857,7 @@
         <v>401</v>
       </c>
       <c r="C547" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
@@ -7132,7 +7132,7 @@
         <v>397</v>
       </c>
       <c r="C572" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
@@ -7143,7 +7143,7 @@
         <v>412</v>
       </c>
       <c r="C573" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
@@ -7418,7 +7418,7 @@
         <v>458</v>
       </c>
       <c r="C598" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
@@ -7429,7 +7429,7 @@
         <v>492</v>
       </c>
       <c r="C599" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
@@ -7704,7 +7704,7 @@
         <v>405</v>
       </c>
       <c r="C624" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.25">
@@ -7715,7 +7715,7 @@
         <v>424</v>
       </c>
       <c r="C625" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.25">
@@ -7990,7 +7990,7 @@
         <v>560</v>
       </c>
       <c r="C650" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
@@ -8001,7 +8001,7 @@
         <v>570</v>
       </c>
       <c r="C651" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -8276,7 +8276,7 @@
         <v>534</v>
       </c>
       <c r="C676" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
@@ -8287,7 +8287,7 @@
         <v>544</v>
       </c>
       <c r="C677" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
@@ -8562,7 +8562,7 @@
         <v>511</v>
       </c>
       <c r="C702" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.25">
@@ -8573,7 +8573,7 @@
         <v>546</v>
       </c>
       <c r="C703" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.25">
@@ -8848,7 +8848,7 @@
         <v>618</v>
       </c>
       <c r="C728" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.25">
@@ -8859,7 +8859,7 @@
         <v>637</v>
       </c>
       <c r="C729" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.25">
@@ -9134,7 +9134,7 @@
         <v>506</v>
       </c>
       <c r="C754" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
@@ -9145,7 +9145,7 @@
         <v>547</v>
       </c>
       <c r="C755" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
@@ -9420,7 +9420,7 @@
         <v>496</v>
       </c>
       <c r="C780" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
@@ -9431,7 +9431,7 @@
         <v>508</v>
       </c>
       <c r="C781" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
@@ -9706,7 +9706,7 @@
         <v>517</v>
       </c>
       <c r="C806" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.25">
@@ -9717,7 +9717,7 @@
         <v>580</v>
       </c>
       <c r="C807" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">
@@ -9992,7 +9992,7 @@
         <v>562</v>
       </c>
       <c r="C832" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.25">
@@ -10003,7 +10003,7 @@
         <v>586</v>
       </c>
       <c r="C833" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.25">
@@ -10278,7 +10278,7 @@
         <v>476</v>
       </c>
       <c r="C858" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.25">
@@ -10289,7 +10289,7 @@
         <v>544</v>
       </c>
       <c r="C859" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.25">
@@ -10564,7 +10564,7 @@
         <v>468</v>
       </c>
       <c r="C884" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -10575,7 +10575,7 @@
         <v>492</v>
       </c>
       <c r="C885" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.25">
@@ -10850,7 +10850,7 @@
         <v>457</v>
       </c>
       <c r="C910" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.25">
@@ -10861,7 +10861,7 @@
         <v>464</v>
       </c>
       <c r="C911" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.25">
@@ -11136,7 +11136,7 @@
         <v>498</v>
       </c>
       <c r="C936" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="937" spans="1:3" x14ac:dyDescent="0.25">
@@ -11147,7 +11147,7 @@
         <v>571</v>
       </c>
       <c r="C937" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="938" spans="1:3" x14ac:dyDescent="0.25">
@@ -11422,7 +11422,7 @@
         <v>489</v>
       </c>
       <c r="C962" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="963" spans="1:3" x14ac:dyDescent="0.25">
@@ -11433,7 +11433,7 @@
         <v>515</v>
       </c>
       <c r="C963" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="964" spans="1:3" x14ac:dyDescent="0.25">
@@ -11708,7 +11708,7 @@
         <v>399</v>
       </c>
       <c r="C988" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="989" spans="1:3" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>409</v>
       </c>
       <c r="C989" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="990" spans="1:3" x14ac:dyDescent="0.25">
@@ -11994,7 +11994,7 @@
         <v>463</v>
       </c>
       <c r="C1014" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1015" spans="1:3" x14ac:dyDescent="0.25">
@@ -12005,7 +12005,7 @@
         <v>477</v>
       </c>
       <c r="C1015" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1016" spans="1:3" x14ac:dyDescent="0.25">
@@ -12280,7 +12280,7 @@
         <v>427</v>
       </c>
       <c r="C1040" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1041" spans="1:3" x14ac:dyDescent="0.25">
@@ -12291,7 +12291,7 @@
         <v>434</v>
       </c>
       <c r="C1041" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1042" spans="1:3" x14ac:dyDescent="0.25">
@@ -12566,7 +12566,7 @@
         <v>541</v>
       </c>
       <c r="C1066" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1067" spans="1:3" x14ac:dyDescent="0.25">
@@ -12577,7 +12577,7 @@
         <v>542</v>
       </c>
       <c r="C1067" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1068" spans="1:3" x14ac:dyDescent="0.25">
@@ -12852,7 +12852,7 @@
         <v>432</v>
       </c>
       <c r="C1092" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1093" spans="1:3" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>432</v>
       </c>
       <c r="C1093" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1094" spans="1:3" x14ac:dyDescent="0.25">
@@ -13138,7 +13138,7 @@
         <v>594</v>
       </c>
       <c r="C1118" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1119" spans="1:3" x14ac:dyDescent="0.25">
@@ -13149,7 +13149,7 @@
         <v>651</v>
       </c>
       <c r="C1119" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1120" spans="1:3" x14ac:dyDescent="0.25">
@@ -13424,7 +13424,7 @@
         <v>395</v>
       </c>
       <c r="C1144" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1145" spans="1:3" x14ac:dyDescent="0.25">
@@ -13435,7 +13435,7 @@
         <v>409</v>
       </c>
       <c r="C1145" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1146" spans="1:3" x14ac:dyDescent="0.25">
@@ -13710,7 +13710,7 @@
         <v>410</v>
       </c>
       <c r="C1170" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1171" spans="1:3" x14ac:dyDescent="0.25">
@@ -13721,7 +13721,7 @@
         <v>425</v>
       </c>
       <c r="C1171" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1172" spans="1:3" x14ac:dyDescent="0.25">
@@ -13996,7 +13996,7 @@
         <v>383</v>
       </c>
       <c r="C1196" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1197" spans="1:3" x14ac:dyDescent="0.25">
@@ -14007,7 +14007,7 @@
         <v>403</v>
       </c>
       <c r="C1197" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1198" spans="1:3" x14ac:dyDescent="0.25">
@@ -14282,7 +14282,7 @@
         <v>566</v>
       </c>
       <c r="C1222" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1223" spans="1:3" x14ac:dyDescent="0.25">
@@ -14293,7 +14293,7 @@
         <v>635</v>
       </c>
       <c r="C1223" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1224" spans="1:3" x14ac:dyDescent="0.25">
@@ -14568,7 +14568,7 @@
         <v>570</v>
       </c>
       <c r="C1248" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1249" spans="1:3" x14ac:dyDescent="0.25">
@@ -14579,7 +14579,7 @@
         <v>581</v>
       </c>
       <c r="C1249" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1250" spans="1:3" x14ac:dyDescent="0.25">
@@ -14854,7 +14854,7 @@
         <v>442</v>
       </c>
       <c r="C1274" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1275" spans="1:3" x14ac:dyDescent="0.25">
@@ -14865,7 +14865,7 @@
         <v>456</v>
       </c>
       <c r="C1275" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1276" spans="1:3" x14ac:dyDescent="0.25">
@@ -15140,7 +15140,7 @@
         <v>541</v>
       </c>
       <c r="C1300" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1301" spans="1:3" x14ac:dyDescent="0.25">
@@ -15151,7 +15151,7 @@
         <v>591</v>
       </c>
       <c r="C1301" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1302" spans="1:3" x14ac:dyDescent="0.25">
@@ -15426,7 +15426,7 @@
         <v>454</v>
       </c>
       <c r="C1326" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1327" spans="1:3" x14ac:dyDescent="0.25">
@@ -15437,7 +15437,7 @@
         <v>478</v>
       </c>
       <c r="C1327" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1328" spans="1:3" x14ac:dyDescent="0.25">
@@ -15712,7 +15712,7 @@
         <v>411</v>
       </c>
       <c r="C1352" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1353" spans="1:3" x14ac:dyDescent="0.25">
@@ -15723,7 +15723,7 @@
         <v>426</v>
       </c>
       <c r="C1353" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1354" spans="1:3" x14ac:dyDescent="0.25">
@@ -15998,7 +15998,7 @@
         <v>472</v>
       </c>
       <c r="C1378" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1379" spans="1:3" x14ac:dyDescent="0.25">
@@ -16009,7 +16009,7 @@
         <v>496</v>
       </c>
       <c r="C1379" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1380" spans="1:3" x14ac:dyDescent="0.25">
@@ -16284,7 +16284,7 @@
         <v>405</v>
       </c>
       <c r="C1404" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1405" spans="1:3" x14ac:dyDescent="0.25">
@@ -16295,7 +16295,7 @@
         <v>416</v>
       </c>
       <c r="C1405" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1406" spans="1:3" x14ac:dyDescent="0.25">
@@ -16570,7 +16570,7 @@
         <v>420</v>
       </c>
       <c r="C1430" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1431" spans="1:3" x14ac:dyDescent="0.25">
@@ -16581,7 +16581,7 @@
         <v>435</v>
       </c>
       <c r="C1431" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1432" spans="1:3" x14ac:dyDescent="0.25">
@@ -16856,7 +16856,7 @@
         <v>394</v>
       </c>
       <c r="C1456" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1457" spans="1:3" x14ac:dyDescent="0.25">
@@ -16867,7 +16867,7 @@
         <v>404</v>
       </c>
       <c r="C1457" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1458" spans="1:3" x14ac:dyDescent="0.25">
@@ -17142,7 +17142,7 @@
         <v>439</v>
       </c>
       <c r="C1482" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1483" spans="1:3" x14ac:dyDescent="0.25">
@@ -17153,7 +17153,7 @@
         <v>449</v>
       </c>
       <c r="C1483" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1484" spans="1:3" x14ac:dyDescent="0.25">
@@ -17428,7 +17428,7 @@
         <v>541</v>
       </c>
       <c r="C1508" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1509" spans="1:3" x14ac:dyDescent="0.25">
@@ -17439,7 +17439,7 @@
         <v>560</v>
       </c>
       <c r="C1509" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1510" spans="1:3" x14ac:dyDescent="0.25">
@@ -17714,7 +17714,7 @@
         <v>440</v>
       </c>
       <c r="C1534" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1535" spans="1:3" x14ac:dyDescent="0.25">
@@ -17725,7 +17725,7 @@
         <v>463</v>
       </c>
       <c r="C1535" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1536" spans="1:3" x14ac:dyDescent="0.25">
@@ -18000,7 +18000,7 @@
         <v>525</v>
       </c>
       <c r="C1560" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1561" spans="1:3" x14ac:dyDescent="0.25">
@@ -18011,7 +18011,7 @@
         <v>539</v>
       </c>
       <c r="C1561" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1562" spans="1:3" x14ac:dyDescent="0.25">
@@ -18286,7 +18286,7 @@
         <v>393</v>
       </c>
       <c r="C1586" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1587" spans="1:3" x14ac:dyDescent="0.25">
@@ -18297,7 +18297,7 @@
         <v>406</v>
       </c>
       <c r="C1587" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1588" spans="1:3" x14ac:dyDescent="0.25">
@@ -18572,7 +18572,7 @@
         <v>504</v>
       </c>
       <c r="C1612" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1613" spans="1:3" x14ac:dyDescent="0.25">
@@ -18583,7 +18583,7 @@
         <v>525</v>
       </c>
       <c r="C1613" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1614" spans="1:3" x14ac:dyDescent="0.25">
@@ -18858,7 +18858,7 @@
         <v>406</v>
       </c>
       <c r="C1638" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1639" spans="1:3" x14ac:dyDescent="0.25">
@@ -18869,7 +18869,7 @@
         <v>421</v>
       </c>
       <c r="C1639" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1640" spans="1:3" x14ac:dyDescent="0.25">
@@ -19144,7 +19144,7 @@
         <v>480</v>
       </c>
       <c r="C1664" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1665" spans="1:3" x14ac:dyDescent="0.25">
@@ -19155,7 +19155,7 @@
         <v>493</v>
       </c>
       <c r="C1665" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1666" spans="1:3" x14ac:dyDescent="0.25">
@@ -19430,7 +19430,7 @@
         <v>471</v>
       </c>
       <c r="C1690" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1691" spans="1:3" x14ac:dyDescent="0.25">
@@ -19441,7 +19441,7 @@
         <v>482</v>
       </c>
       <c r="C1691" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1692" spans="1:3" x14ac:dyDescent="0.25">
@@ -19716,7 +19716,7 @@
         <v>478</v>
       </c>
       <c r="C1716" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1717" spans="1:3" x14ac:dyDescent="0.25">
@@ -19727,7 +19727,7 @@
         <v>484</v>
       </c>
       <c r="C1717" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1718" spans="1:3" x14ac:dyDescent="0.25">
@@ -20002,7 +20002,7 @@
         <v>542</v>
       </c>
       <c r="C1742" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1743" spans="1:3" x14ac:dyDescent="0.25">
@@ -20013,7 +20013,7 @@
         <v>555</v>
       </c>
       <c r="C1743" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1744" spans="1:3" x14ac:dyDescent="0.25">
@@ -20288,7 +20288,7 @@
         <v>633</v>
       </c>
       <c r="C1768" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1769" spans="1:3" x14ac:dyDescent="0.25">
@@ -20299,7 +20299,7 @@
         <v>655</v>
       </c>
       <c r="C1769" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1770" spans="1:3" x14ac:dyDescent="0.25">
@@ -20574,7 +20574,7 @@
         <v>391</v>
       </c>
       <c r="C1794" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1795" spans="1:3" x14ac:dyDescent="0.25">
@@ -20585,7 +20585,7 @@
         <v>401</v>
       </c>
       <c r="C1795" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1796" spans="1:3" x14ac:dyDescent="0.25">
@@ -20860,7 +20860,7 @@
         <v>396</v>
       </c>
       <c r="C1820" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1821" spans="1:3" x14ac:dyDescent="0.25">
@@ -20871,7 +20871,7 @@
         <v>409</v>
       </c>
       <c r="C1821" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1822" spans="1:3" x14ac:dyDescent="0.25">
@@ -21146,7 +21146,7 @@
         <v>463</v>
       </c>
       <c r="C1846" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1847" spans="1:3" x14ac:dyDescent="0.25">
@@ -21157,7 +21157,7 @@
         <v>478</v>
       </c>
       <c r="C1847" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1848" spans="1:3" x14ac:dyDescent="0.25">
@@ -21432,7 +21432,7 @@
         <v>383</v>
       </c>
       <c r="C1872" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1873" spans="1:3" x14ac:dyDescent="0.25">
@@ -21443,7 +21443,7 @@
         <v>396</v>
       </c>
       <c r="C1873" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1874" spans="1:3" x14ac:dyDescent="0.25">
@@ -21718,7 +21718,7 @@
         <v>552</v>
       </c>
       <c r="C1898" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1899" spans="1:3" x14ac:dyDescent="0.25">
@@ -21729,7 +21729,7 @@
         <v>612</v>
       </c>
       <c r="C1899" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1900" spans="1:3" x14ac:dyDescent="0.25">
@@ -22004,7 +22004,7 @@
         <v>554</v>
       </c>
       <c r="C1924" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1925" spans="1:3" x14ac:dyDescent="0.25">
@@ -22015,7 +22015,7 @@
         <v>590</v>
       </c>
       <c r="C1925" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1926" spans="1:3" x14ac:dyDescent="0.25">
@@ -22290,7 +22290,7 @@
         <v>459</v>
       </c>
       <c r="C1950" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1951" spans="1:3" x14ac:dyDescent="0.25">
@@ -22301,7 +22301,7 @@
         <v>468</v>
       </c>
       <c r="C1951" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1952" spans="1:3" x14ac:dyDescent="0.25">
@@ -22576,7 +22576,7 @@
         <v>497</v>
       </c>
       <c r="C1976" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="1977" spans="1:3" x14ac:dyDescent="0.25">
@@ -22587,7 +22587,7 @@
         <v>527</v>
       </c>
       <c r="C1977" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1978" spans="1:3" x14ac:dyDescent="0.25">
@@ -22862,7 +22862,7 @@
         <v>388</v>
       </c>
       <c r="C2002" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2003" spans="1:3" x14ac:dyDescent="0.25">
@@ -22873,7 +22873,7 @@
         <v>397</v>
       </c>
       <c r="C2003" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2004" spans="1:3" x14ac:dyDescent="0.25">
@@ -23148,7 +23148,7 @@
         <v>542</v>
       </c>
       <c r="C2028" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2029" spans="1:3" x14ac:dyDescent="0.25">
@@ -23159,7 +23159,7 @@
         <v>554</v>
       </c>
       <c r="C2029" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2030" spans="1:3" x14ac:dyDescent="0.25">
@@ -23434,7 +23434,7 @@
         <v>442</v>
       </c>
       <c r="C2054" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2055" spans="1:3" x14ac:dyDescent="0.25">
@@ -23445,7 +23445,7 @@
         <v>475</v>
       </c>
       <c r="C2055" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2056" spans="1:3" x14ac:dyDescent="0.25">
@@ -23720,7 +23720,7 @@
         <v>450</v>
       </c>
       <c r="C2080" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2081" spans="1:3" x14ac:dyDescent="0.25">
@@ -23731,7 +23731,7 @@
         <v>463</v>
       </c>
       <c r="C2081" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2082" spans="1:3" x14ac:dyDescent="0.25">
@@ -24006,7 +24006,7 @@
         <v>465</v>
       </c>
       <c r="C2106" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2107" spans="1:3" x14ac:dyDescent="0.25">
@@ -24017,7 +24017,7 @@
         <v>479</v>
       </c>
       <c r="C2107" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2108" spans="1:3" x14ac:dyDescent="0.25">
@@ -24292,7 +24292,7 @@
         <v>465</v>
       </c>
       <c r="C2132" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2133" spans="1:3" x14ac:dyDescent="0.25">
@@ -24303,7 +24303,7 @@
         <v>517</v>
       </c>
       <c r="C2133" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2134" spans="1:3" x14ac:dyDescent="0.25">
@@ -24578,7 +24578,7 @@
         <v>422</v>
       </c>
       <c r="C2158" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2159" spans="1:3" x14ac:dyDescent="0.25">
@@ -24589,7 +24589,7 @@
         <v>436</v>
       </c>
       <c r="C2159" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2160" spans="1:3" x14ac:dyDescent="0.25">
@@ -24864,7 +24864,7 @@
         <v>430</v>
       </c>
       <c r="C2184" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2185" spans="1:3" x14ac:dyDescent="0.25">
@@ -24875,7 +24875,7 @@
         <v>444</v>
       </c>
       <c r="C2185" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2186" spans="1:3" x14ac:dyDescent="0.25">
@@ -25150,7 +25150,7 @@
         <v>470</v>
       </c>
       <c r="C2210" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2211" spans="1:3" x14ac:dyDescent="0.25">
@@ -25161,7 +25161,7 @@
         <v>479</v>
       </c>
       <c r="C2211" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2212" spans="1:3" x14ac:dyDescent="0.25">
@@ -25436,7 +25436,7 @@
         <v>490</v>
       </c>
       <c r="C2236" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2237" spans="1:3" x14ac:dyDescent="0.25">
@@ -25447,7 +25447,7 @@
         <v>516</v>
       </c>
       <c r="C2237" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2238" spans="1:3" x14ac:dyDescent="0.25">
@@ -25722,7 +25722,7 @@
         <v>412</v>
       </c>
       <c r="C2262" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2263" spans="1:3" x14ac:dyDescent="0.25">
@@ -25733,7 +25733,7 @@
         <v>431</v>
       </c>
       <c r="C2263" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2264" spans="1:3" x14ac:dyDescent="0.25">
@@ -26008,7 +26008,7 @@
         <v>445</v>
       </c>
       <c r="C2288" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2289" spans="1:3" x14ac:dyDescent="0.25">
@@ -26019,7 +26019,7 @@
         <v>452</v>
       </c>
       <c r="C2289" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2290" spans="1:3" x14ac:dyDescent="0.25">
@@ -26294,7 +26294,7 @@
         <v>383</v>
       </c>
       <c r="C2314" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2315" spans="1:3" x14ac:dyDescent="0.25">
@@ -26305,7 +26305,7 @@
         <v>393</v>
       </c>
       <c r="C2315" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2316" spans="1:3" x14ac:dyDescent="0.25">
@@ -26580,7 +26580,7 @@
         <v>477</v>
       </c>
       <c r="C2340" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2341" spans="1:3" x14ac:dyDescent="0.25">
@@ -26591,7 +26591,7 @@
         <v>500</v>
       </c>
       <c r="C2341" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2342" spans="1:3" x14ac:dyDescent="0.25">
@@ -26866,7 +26866,7 @@
         <v>490</v>
       </c>
       <c r="C2366" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2367" spans="1:3" x14ac:dyDescent="0.25">
@@ -26877,7 +26877,7 @@
         <v>505</v>
       </c>
       <c r="C2367" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2368" spans="1:3" x14ac:dyDescent="0.25">
@@ -27152,7 +27152,7 @@
         <v>602</v>
       </c>
       <c r="C2392" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2393" spans="1:3" x14ac:dyDescent="0.25">
@@ -27163,7 +27163,7 @@
         <v>615</v>
       </c>
       <c r="C2393" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2394" spans="1:3" x14ac:dyDescent="0.25">
@@ -27438,7 +27438,7 @@
         <v>390</v>
       </c>
       <c r="C2418" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2419" spans="1:3" x14ac:dyDescent="0.25">
@@ -27449,7 +27449,7 @@
         <v>405</v>
       </c>
       <c r="C2419" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2420" spans="1:3" x14ac:dyDescent="0.25">
@@ -27724,7 +27724,7 @@
         <v>417</v>
       </c>
       <c r="C2444" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2445" spans="1:3" x14ac:dyDescent="0.25">
@@ -27735,7 +27735,7 @@
         <v>428</v>
       </c>
       <c r="C2445" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2446" spans="1:3" x14ac:dyDescent="0.25">
@@ -28010,7 +28010,7 @@
         <v>421</v>
       </c>
       <c r="C2470" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2471" spans="1:3" x14ac:dyDescent="0.25">
@@ -28021,7 +28021,7 @@
         <v>431</v>
       </c>
       <c r="C2471" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2472" spans="1:3" x14ac:dyDescent="0.25">
@@ -28296,7 +28296,7 @@
         <v>438</v>
       </c>
       <c r="C2496" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2497" spans="1:3" x14ac:dyDescent="0.25">
@@ -28307,7 +28307,7 @@
         <v>476</v>
       </c>
       <c r="C2497" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2498" spans="1:3" x14ac:dyDescent="0.25">
@@ -28582,7 +28582,7 @@
         <v>480</v>
       </c>
       <c r="C2522" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2523" spans="1:3" x14ac:dyDescent="0.25">
@@ -28593,7 +28593,7 @@
         <v>493</v>
       </c>
       <c r="C2523" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2524" spans="1:3" x14ac:dyDescent="0.25">
@@ -28868,7 +28868,7 @@
         <v>412</v>
       </c>
       <c r="C2548" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2549" spans="1:3" x14ac:dyDescent="0.25">
@@ -28879,7 +28879,7 @@
         <v>423</v>
       </c>
       <c r="C2549" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2550" spans="1:3" x14ac:dyDescent="0.25">
@@ -29154,7 +29154,7 @@
         <v>424</v>
       </c>
       <c r="C2574" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2575" spans="1:3" x14ac:dyDescent="0.25">
@@ -29165,7 +29165,7 @@
         <v>440</v>
       </c>
       <c r="C2575" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2576" spans="1:3" x14ac:dyDescent="0.25">
@@ -29440,7 +29440,7 @@
         <v>383</v>
       </c>
       <c r="C2600" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2601" spans="1:3" x14ac:dyDescent="0.25">
@@ -29451,7 +29451,7 @@
         <v>393</v>
       </c>
       <c r="C2601" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>